<commit_message>
Test that vars are correlated
Increased numreal to 500 for correlated samples in
design_input_background.xlsx

Change PARAM11 from Triangle(1, 1, 1) to Triangle(0, 0.5, 1).
</commit_message>
<xml_diff>
--- a/tests/sensitivities/data/config/design_input_background.xlsx
+++ b/tests/sensitivities/data/config/design_input_background.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F818A72B-633D-8F4D-A600-F8B4ADA22047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFA1221-5FDB-3C4B-BC4E-DD36F86EA8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16340" yWindow="5100" windowWidth="37220" windowHeight="24200" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15380" yWindow="32760" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="background" sheetId="5" r:id="rId5"/>
     <sheet name="background_corr" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2751,7 +2751,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3139,7 +3139,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="145">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="C13" s="146" t="s">
         <v>35</v>
@@ -3215,10 +3215,10 @@
         <v>45</v>
       </c>
       <c r="J15" s="151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="152">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L15" s="153">
         <v>1</v>
@@ -3590,7 +3590,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" activeCellId="1" sqref="C1 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>